<commit_message>
Finish sample BDD test cases Implementing GUI tests
</commit_message>
<xml_diff>
--- a/P1.3 - Bug Report.xlsx
+++ b/P1.3 - Bug Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Doing submit form with empty keyword returns "London, UK" result with empty data</t>
-  </si>
-  <si>
-    <t>Bad UX behavior, the "magnifying" icon should be designed as a submit button (with friendly tooltip such as "Click here to submit"</t>
   </si>
   <si>
     <t>High</t>
@@ -240,6 +237,10 @@
   </si>
   <si>
     <t>Count of #</t>
+  </si>
+  <si>
+    <t>Looks like submit button is hidden
+Bad UX behavior, the "magnifying" icon should be designed as a submit button (with friendly tooltip such as "Click here to submit"</t>
   </si>
 </sst>
 </file>
@@ -477,11 +478,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="84914560"/>
-        <c:axId val="84916096"/>
+        <c:axId val="76898688"/>
+        <c:axId val="76900224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84914560"/>
+        <c:axId val="76898688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84916096"/>
+        <c:crossAx val="76900224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,7 +499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84916096"/>
+        <c:axId val="76900224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84914560"/>
+        <c:crossAx val="76898688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -943,7 +944,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A2:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -1035,19 +1036,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G40" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G40" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G40"/>
-  <sortState ref="A2:G40">
-    <sortCondition ref="D1:D40"/>
+  <sortState ref="A2:G22">
+    <sortCondition ref="E1:E40"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="8"/>
-    <tableColumn id="2" name="Summary" dataDxfId="7"/>
-    <tableColumn id="3" name="Area" dataDxfId="6"/>
-    <tableColumn id="4" name="Priority" dataDxfId="5"/>
-    <tableColumn id="5" name="Severity" dataDxfId="4"/>
-    <tableColumn id="7" name="Triage comment" dataDxfId="3"/>
-    <tableColumn id="8" name="Note" dataDxfId="2"/>
+    <tableColumn id="1" name="#" dataDxfId="6"/>
+    <tableColumn id="2" name="Summary" dataDxfId="5"/>
+    <tableColumn id="3" name="Area" dataDxfId="4"/>
+    <tableColumn id="4" name="Priority" dataDxfId="3"/>
+    <tableColumn id="5" name="Severity" dataDxfId="2"/>
+    <tableColumn id="7" name="Triage comment" dataDxfId="1"/>
+    <tableColumn id="8" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1342,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1359,10 +1360,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1375,7 +1376,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -1391,7 +1392,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4">
         <v>12</v>
@@ -1399,7 +1400,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4">
         <v>4</v>
@@ -1407,7 +1408,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4">
         <v>5</v>
@@ -1423,7 +1424,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4">
         <v>21</v>
@@ -1439,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,165 +1485,165 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -1650,107 +1651,107 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
@@ -1762,58 +1763,55 @@
         <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
@@ -1825,15 +1823,18 @@
         <v>9</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>8</v>
@@ -1842,21 +1843,21 @@
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
@@ -1865,18 +1866,18 @@
         <v>9</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
@@ -1885,18 +1886,18 @@
         <v>9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>10</v>
@@ -1905,7 +1906,7 @@
         <v>9</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>